<commit_message>
Fixed FlexDemands (EV charging must be 0 if not connected)
</commit_message>
<xml_diff>
--- a/data/input/Example_building_opt.xlsx
+++ b/data/input/Example_building_opt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\PycharmProjects\P2Bldg\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40724A8C-E4EB-42D2-96B9-BBFD5830C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB28DD1-6A6C-4517-A76F-7F85A58A61FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{61AF8562-6E46-4D5E-8B33-C109B79F9DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{61AF8562-6E46-4D5E-8B33-C109B79F9DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -10125,8 +10125,8 @@
   </sheetPr>
   <dimension ref="A1:O187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
@@ -15475,8 +15475,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>